<commit_message>
Truckloads of work on map, plot, cinematics, and sequence. The game is pretty playable and tested through level 15~ right now (Robo Water Weird boss) and has a bunch of cinematics. Lots of balance work on mob stats as well as player abilities. Rearranged some class abilities to be better suited, and added a bunch of new abilities to flesh out the leveling progression.
</commit_message>
<xml_diff>
--- a/Progression.xlsx
+++ b/Progression.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\TME_RPG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Polatrite\Dropbox\TME_RPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9960" tabRatio="834" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18768" windowHeight="9960" tabRatio="834" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Area Progression" sheetId="1" r:id="rId1"/>
@@ -251,13 +251,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,14 +544,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -562,7 +562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -573,7 +573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -584,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>9</v>
       </c>
@@ -595,7 +595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>16</v>
       </c>
@@ -606,7 +606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>23</v>
       </c>
@@ -617,7 +617,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>31</v>
       </c>
@@ -628,7 +628,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>38</v>
       </c>
@@ -639,7 +639,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>46</v>
       </c>
@@ -664,41 +664,41 @@
       <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="23"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="7"/>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="23"/>
+      <c r="I1" s="27"/>
       <c r="J1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="K1" s="7"/>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="23"/>
+      <c r="M1" s="27"/>
       <c r="N1" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -742,7 +742,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <f t="shared" ref="B3:N3" si="0">(B5-B4)/50</f>
         <v>28.8</v>
@@ -796,7 +796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -840,7 +840,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>51</v>
       </c>
@@ -884,7 +884,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -941,7 +941,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>3</v>
       </c>
@@ -998,7 +998,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>10</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1796,7 +1796,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>20</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>21</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>22</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>23</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>24</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>25</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>26</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>27</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>28</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>29</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>30</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>31</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>32</v>
       </c>
@@ -2651,7 +2651,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>33</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>34</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>35</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>36</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>37</v>
       </c>
@@ -2936,7 +2936,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>38</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>39</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>40</v>
       </c>
@@ -3107,7 +3107,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>41</v>
       </c>
@@ -3164,7 +3164,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>42</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>43</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>44</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>45</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>46</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>47</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>48</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>49</v>
       </c>
@@ -3620,7 +3620,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>50</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>51</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -3749,7 +3749,7 @@
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>51</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>52</v>
       </c>
@@ -3853,48 +3853,49 @@
   <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <pane ySplit="3024" topLeftCell="A50" activePane="bottomLeft"/>
+      <selection activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="19"/>
+    <col min="1" max="1" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="23"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="7"/>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="23"/>
+      <c r="I1" s="27"/>
       <c r="J1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="K1" s="7"/>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="23"/>
+      <c r="M1" s="27"/>
       <c r="N1" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>22</v>
       </c>
@@ -3938,7 +3939,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19"/>
       <c r="B3" s="10" t="s">
         <v>12</v>
@@ -3974,7 +3975,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="19"/>
       <c r="B4" s="10" t="s">
         <v>23</v>
@@ -3994,13 +3995,13 @@
         <v>23</v>
       </c>
       <c r="I4" s="17">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>23</v>
@@ -4010,7 +4011,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
       <c r="B5" s="10" t="s">
         <v>24</v>
@@ -4036,7 +4037,7 @@
         <v>24</v>
       </c>
       <c r="K5" s="14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>24</v>
@@ -4046,7 +4047,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="10" t="s">
         <v>25</v>
@@ -4066,7 +4067,7 @@
         <v>25</v>
       </c>
       <c r="I6" s="17">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>25</v>
@@ -4080,7 +4081,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
       <c r="B7" s="10" t="s">
         <v>26</v>
@@ -4097,11 +4098,15 @@
       <c r="H7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="16"/>
+      <c r="I7" s="17">
+        <v>0.2</v>
+      </c>
       <c r="J7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="15"/>
+      <c r="K7" s="14">
+        <v>0.2</v>
+      </c>
       <c r="L7" s="10" t="s">
         <v>26</v>
       </c>
@@ -4110,7 +4115,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="19"/>
       <c r="B8" s="10" t="s">
         <v>27</v>
@@ -4146,7 +4151,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
       <c r="B9" s="10" t="s">
         <v>28</v>
@@ -4179,7 +4184,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19"/>
       <c r="C10" s="11"/>
       <c r="E10" s="11"/>
@@ -4188,7 +4193,7 @@
       <c r="K10" s="12"/>
       <c r="M10" s="11"/>
     </row>
-    <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="20"/>
       <c r="B11" s="2">
         <f t="shared" ref="B11:N11" si="0">(B13-B12)/50</f>
@@ -4243,7 +4248,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
         <v>1</v>
       </c>
@@ -4287,7 +4292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="21">
         <v>51</v>
       </c>
@@ -4331,7 +4336,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>2</v>
       </c>
@@ -4388,7 +4393,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>3</v>
       </c>
@@ -4445,7 +4450,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>4</v>
       </c>
@@ -4502,7 +4507,7 @@
         <v>1.7999999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>5</v>
       </c>
@@ -4559,7 +4564,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>6</v>
       </c>
@@ -4616,7 +4621,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>7</v>
       </c>
@@ -4673,7 +4678,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>8</v>
       </c>
@@ -4730,7 +4735,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="19">
         <v>9</v>
       </c>
@@ -4787,7 +4792,7 @@
         <v>4.8</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>10</v>
       </c>
@@ -4844,7 +4849,7 @@
         <v>5.3999999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>11</v>
       </c>
@@ -4901,7 +4906,7 @@
         <v>5.9999999999999991</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>12</v>
       </c>
@@ -4958,7 +4963,7 @@
         <v>6.5999999999999988</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>13</v>
       </c>
@@ -5015,7 +5020,7 @@
         <v>7.1999999999999984</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>14</v>
       </c>
@@ -5072,7 +5077,7 @@
         <v>7.799999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>15</v>
       </c>
@@ -5129,7 +5134,7 @@
         <v>8.3999999999999986</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>16</v>
       </c>
@@ -5186,7 +5191,7 @@
         <v>8.9999999999999982</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>17</v>
       </c>
@@ -5243,7 +5248,7 @@
         <v>9.5999999999999979</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <v>18</v>
       </c>
@@ -5300,7 +5305,7 @@
         <v>10.199999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="19">
         <v>19</v>
       </c>
@@ -5357,7 +5362,7 @@
         <v>10.799999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="19">
         <v>20</v>
       </c>
@@ -5414,7 +5419,7 @@
         <v>11.399999999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <v>21</v>
       </c>
@@ -5471,7 +5476,7 @@
         <v>11.999999999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
         <v>22</v>
       </c>
@@ -5528,7 +5533,7 @@
         <v>12.599999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="19">
         <v>23</v>
       </c>
@@ -5585,7 +5590,7 @@
         <v>13.199999999999996</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="19">
         <v>24</v>
       </c>
@@ -5642,7 +5647,7 @@
         <v>13.799999999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="19">
         <v>25</v>
       </c>
@@ -5699,7 +5704,7 @@
         <v>14.399999999999995</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="19">
         <v>26</v>
       </c>
@@ -5756,7 +5761,7 @@
         <v>14.999999999999995</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="19">
         <v>27</v>
       </c>
@@ -5813,7 +5818,7 @@
         <v>15.599999999999994</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
         <v>28</v>
       </c>
@@ -5870,7 +5875,7 @@
         <v>16.199999999999996</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="19">
         <v>29</v>
       </c>
@@ -5927,7 +5932,7 @@
         <v>16.799999999999997</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="19">
         <v>30</v>
       </c>
@@ -5984,7 +5989,7 @@
         <v>17.399999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="19">
         <v>31</v>
       </c>
@@ -6041,7 +6046,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="19">
         <v>32</v>
       </c>
@@ -6098,7 +6103,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="19">
         <v>33</v>
       </c>
@@ -6155,7 +6160,7 @@
         <v>19.200000000000003</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="19">
         <v>34</v>
       </c>
@@ -6212,7 +6217,7 @@
         <v>19.800000000000004</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <v>35</v>
       </c>
@@ -6269,7 +6274,7 @@
         <v>20.400000000000006</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="19">
         <v>36</v>
       </c>
@@ -6326,7 +6331,7 @@
         <v>21.000000000000007</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="19">
         <v>37</v>
       </c>
@@ -6383,7 +6388,7 @@
         <v>21.600000000000009</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="19">
         <v>38</v>
       </c>
@@ -6440,7 +6445,7 @@
         <v>22.20000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="19">
         <v>39</v>
       </c>
@@ -6497,7 +6502,7 @@
         <v>22.800000000000011</v>
       </c>
     </row>
-    <row r="52" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="19">
         <v>40</v>
       </c>
@@ -6554,7 +6559,7 @@
         <v>23.400000000000013</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="19">
         <v>41</v>
       </c>
@@ -6611,7 +6616,7 @@
         <v>24.000000000000014</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="19">
         <v>42</v>
       </c>
@@ -6668,7 +6673,7 @@
         <v>24.600000000000016</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="19">
         <v>43</v>
       </c>
@@ -6725,7 +6730,7 @@
         <v>25.200000000000017</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="19">
         <v>44</v>
       </c>
@@ -6782,7 +6787,7 @@
         <v>25.800000000000018</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="19">
         <v>45</v>
       </c>
@@ -6839,7 +6844,7 @@
         <v>26.40000000000002</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="19">
         <v>46</v>
       </c>
@@ -6896,7 +6901,7 @@
         <v>27.000000000000021</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="19">
         <v>47</v>
       </c>
@@ -6953,7 +6958,7 @@
         <v>27.600000000000023</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="19">
         <v>48</v>
       </c>
@@ -7010,7 +7015,7 @@
         <v>28.200000000000024</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="19">
         <v>49</v>
       </c>
@@ -7067,7 +7072,7 @@
         <v>28.800000000000026</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="19">
         <v>50</v>
       </c>
@@ -7124,7 +7129,7 @@
         <v>29.400000000000027</v>
       </c>
     </row>
-    <row r="63" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63" s="19">
         <v>51</v>
       </c>
@@ -7181,7 +7186,7 @@
         <v>30.000000000000028</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -7217,41 +7222,41 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="23"/>
+      <c r="C1" s="27"/>
       <c r="D1" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="7"/>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23" t="s">
+      <c r="G1" s="27"/>
+      <c r="H1" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="23"/>
+      <c r="I1" s="27"/>
       <c r="J1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="K1" s="7"/>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="23"/>
+      <c r="M1" s="27"/>
       <c r="N1" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
@@ -7295,7 +7300,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -7352,7 +7357,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -7409,7 +7414,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -7466,7 +7471,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -7523,7 +7528,7 @@
         <v>31.8</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -7580,7 +7585,7 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -7637,7 +7642,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -7694,7 +7699,7 @@
         <v>33.6</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>8</v>
       </c>
@@ -7751,7 +7756,7 @@
         <v>34.200000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>9</v>
       </c>
@@ -7808,7 +7813,7 @@
         <v>34.799999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -7865,7 +7870,7 @@
         <v>35.4</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -7922,7 +7927,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -7979,7 +7984,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>13</v>
       </c>
@@ -8036,7 +8041,7 @@
         <v>37.199999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -8093,7 +8098,7 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>15</v>
       </c>
@@ -8150,7 +8155,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -8207,7 +8212,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>17</v>
       </c>
@@ -8264,7 +8269,7 @@
         <v>39.599999999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -8321,7 +8326,7 @@
         <v>40.199999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>19</v>
       </c>
@@ -8378,7 +8383,7 @@
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -8435,7 +8440,7 @@
         <v>41.4</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -8492,7 +8497,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>22</v>
       </c>
@@ -8549,7 +8554,7 @@
         <v>42.599999999999994</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>23</v>
       </c>
@@ -8606,7 +8611,7 @@
         <v>43.199999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>24</v>
       </c>
@@ -8663,7 +8668,7 @@
         <v>43.8</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>25</v>
       </c>
@@ -8720,7 +8725,7 @@
         <v>44.399999999999991</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>26</v>
       </c>
@@ -8777,7 +8782,7 @@
         <v>44.999999999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>27</v>
       </c>
@@ -8834,7 +8839,7 @@
         <v>45.599999999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>28</v>
       </c>
@@ -8891,7 +8896,7 @@
         <v>46.199999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>29</v>
       </c>
@@ -8948,7 +8953,7 @@
         <v>46.8</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -9005,7 +9010,7 @@
         <v>47.4</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <v>31</v>
       </c>
@@ -9062,7 +9067,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10">
         <v>32</v>
       </c>
@@ -9119,7 +9124,7 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10">
         <v>33</v>
       </c>
@@ -9176,7 +9181,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10">
         <v>34</v>
       </c>
@@ -9233,7 +9238,7 @@
         <v>49.800000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10">
         <v>35</v>
       </c>
@@ -9290,7 +9295,7 @@
         <v>50.400000000000006</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10">
         <v>36</v>
       </c>
@@ -9347,7 +9352,7 @@
         <v>51.000000000000007</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10">
         <v>37</v>
       </c>
@@ -9404,7 +9409,7 @@
         <v>51.600000000000009</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10">
         <v>38</v>
       </c>
@@ -9461,7 +9466,7 @@
         <v>52.20000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10">
         <v>39</v>
       </c>
@@ -9518,7 +9523,7 @@
         <v>52.800000000000011</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -9575,7 +9580,7 @@
         <v>53.400000000000013</v>
       </c>
     </row>
-    <row r="43" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10">
         <v>41</v>
       </c>
@@ -9632,7 +9637,7 @@
         <v>54.000000000000014</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10">
         <v>42</v>
       </c>
@@ -9689,7 +9694,7 @@
         <v>54.600000000000016</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="10">
         <v>43</v>
       </c>
@@ -9746,7 +9751,7 @@
         <v>55.200000000000017</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10">
         <v>44</v>
       </c>
@@ -9803,7 +9808,7 @@
         <v>55.800000000000018</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="10">
         <v>45</v>
       </c>
@@ -9860,7 +9865,7 @@
         <v>56.40000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10">
         <v>46</v>
       </c>
@@ -9917,7 +9922,7 @@
         <v>57.000000000000021</v>
       </c>
     </row>
-    <row r="49" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="10">
         <v>47</v>
       </c>
@@ -9974,7 +9979,7 @@
         <v>57.600000000000023</v>
       </c>
     </row>
-    <row r="50" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10">
         <v>48</v>
       </c>
@@ -10031,7 +10036,7 @@
         <v>58.200000000000024</v>
       </c>
     </row>
-    <row r="51" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="10">
         <v>49</v>
       </c>
@@ -10088,7 +10093,7 @@
         <v>58.800000000000026</v>
       </c>
     </row>
-    <row r="52" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10">
         <v>50</v>
       </c>
@@ -10145,7 +10150,7 @@
         <v>59.400000000000027</v>
       </c>
     </row>
-    <row r="53" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -10202,7 +10207,7 @@
         <v>60.000000000000028</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -10234,39 +10239,39 @@
   <dimension ref="A1:P54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>36</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>37</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="23"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="18" t="s">
         <v>39</v>
       </c>
@@ -10274,20 +10279,20 @@
         <v>14</v>
       </c>
       <c r="J1" s="7"/>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="23"/>
+      <c r="L1" s="27"/>
       <c r="M1" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="6" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="D2" s="24"/>
+      <c r="B2" s="23"/>
+      <c r="D2" s="23"/>
       <c r="F2" s="6" t="s">
         <v>35</v>
       </c>
@@ -10310,17 +10315,17 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="25">
+      <c r="B3" s="24">
         <v>1.5</v>
       </c>
       <c r="C3" s="8">
         <v>3</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="24">
         <v>2</v>
       </c>
       <c r="E3" s="8">
@@ -10339,12 +10344,12 @@
         <v>8</v>
       </c>
       <c r="I3" s="9">
-        <f>('Composite Stats'!$B3+'Composite Stats'!$C3)/2/$H3</f>
-        <v>31.25</v>
+        <f>('Composite Stats'!$B3+'Composite Stats'!$C3+'Base Stat Progression'!A4+'Base Stat Progression'!B4)/4/$H3</f>
+        <v>20.65625</v>
       </c>
       <c r="J3" s="9">
-        <f>('Composite Stats'!$B3+'Composite Stats'!$C3)/2/$H3*1.5</f>
-        <v>46.875</v>
+        <f>('Composite Stats'!$B3+'Composite Stats'!$C3+'Base Stat Progression'!B4+'Base Stat Progression'!C4)/4/$H3*1.5</f>
+        <v>44.53125</v>
       </c>
       <c r="K3" s="9">
         <f>('Composite Stats'!$B3+'Composite Stats'!$C3)/2/$H3</f>
@@ -10359,17 +10364,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="24">
         <v>1.5</v>
       </c>
       <c r="C4" s="8">
         <v>3</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="24">
         <v>2</v>
       </c>
       <c r="E4" s="8">
@@ -10388,12 +10393,12 @@
         <v>8</v>
       </c>
       <c r="I4" s="9">
-        <f>('Composite Stats'!$B4+'Composite Stats'!$C4)/2/$H4</f>
-        <v>39.25</v>
+        <f>('Composite Stats'!$B4+'Composite Stats'!$C4+'Base Stat Progression'!$B6+'Base Stat Progression'!$C6)/4/$H4</f>
+        <v>36.28125</v>
       </c>
       <c r="J4" s="9">
-        <f>('Composite Stats'!$B4+'Composite Stats'!$C4)/2/$H4*1.5</f>
-        <v>58.875</v>
+        <f>('Composite Stats'!$B4+'Composite Stats'!$C4+'Base Stat Progression'!$B6+'Base Stat Progression'!$C6)/4/$H4*1.5</f>
+        <v>54.421875</v>
       </c>
       <c r="K4" s="9">
         <f>('Composite Stats'!$B4+'Composite Stats'!$C4)/2/$H4</f>
@@ -10408,17 +10413,17 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="24">
         <v>1.5</v>
       </c>
       <c r="C5" s="8">
         <v>3</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="24">
         <v>2</v>
       </c>
       <c r="E5" s="8">
@@ -10437,12 +10442,12 @@
         <v>8</v>
       </c>
       <c r="I5" s="9">
-        <f>('Composite Stats'!$B5+'Composite Stats'!$C5)/2/$H5</f>
-        <v>47.25</v>
+        <f>('Composite Stats'!$B5+'Composite Stats'!$C5+'Base Stat Progression'!$B7+'Base Stat Progression'!$C7)/4/$H5</f>
+        <v>42.875</v>
       </c>
       <c r="J5" s="9">
-        <f>('Composite Stats'!$B5+'Composite Stats'!$C5)/2/$H5*1.5</f>
-        <v>70.875</v>
+        <f>('Composite Stats'!$B5+'Composite Stats'!$C5+'Base Stat Progression'!$B7+'Base Stat Progression'!$C7)/4/$H5*1.5</f>
+        <v>64.3125</v>
       </c>
       <c r="K5" s="9">
         <f>('Composite Stats'!$B5+'Composite Stats'!$C5)/2/$H5</f>
@@ -10457,17 +10462,17 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="24">
         <v>1.5</v>
       </c>
       <c r="C6" s="8">
         <v>3</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="24">
         <v>2</v>
       </c>
       <c r="E6" s="8">
@@ -10486,12 +10491,12 @@
         <v>8</v>
       </c>
       <c r="I6" s="9">
-        <f>('Composite Stats'!$B6+'Composite Stats'!$C6)/2/$H6</f>
-        <v>55.25</v>
+        <f>('Composite Stats'!$B6+'Composite Stats'!$C6+'Base Stat Progression'!$B8+'Base Stat Progression'!$C8)/4/$H6</f>
+        <v>49.46875</v>
       </c>
       <c r="J6" s="9">
-        <f>('Composite Stats'!$B6+'Composite Stats'!$C6)/2/$H6*1.5</f>
-        <v>82.875</v>
+        <f>('Composite Stats'!$B6+'Composite Stats'!$C6+'Base Stat Progression'!$B8+'Base Stat Progression'!$C8)/4/$H6*1.5</f>
+        <v>74.203125</v>
       </c>
       <c r="K6" s="9">
         <f>('Composite Stats'!$B6+'Composite Stats'!$C6)/2/$H6</f>
@@ -10506,17 +10511,17 @@
         <v>31.8</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="25">
+      <c r="B7" s="24">
         <v>1.5</v>
       </c>
       <c r="C7" s="8">
         <v>3</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="24">
         <v>2</v>
       </c>
       <c r="E7" s="8">
@@ -10535,12 +10540,12 @@
         <v>7</v>
       </c>
       <c r="I7" s="9">
-        <f>('Composite Stats'!$B7+'Composite Stats'!$C7)/2/$H7</f>
-        <v>72.285714285714292</v>
+        <f>('Composite Stats'!$B7+'Composite Stats'!$C7+'Base Stat Progression'!$B9+'Base Stat Progression'!$C9)/4/$H7</f>
+        <v>64.071428571428569</v>
       </c>
       <c r="J7" s="9">
-        <f>('Composite Stats'!$B7+'Composite Stats'!$C7)/2/$H7*1.5</f>
-        <v>108.42857142857144</v>
+        <f>('Composite Stats'!$B7+'Composite Stats'!$C7+'Base Stat Progression'!$B9+'Base Stat Progression'!$C9)/4/$H7*1.5</f>
+        <v>96.107142857142861</v>
       </c>
       <c r="K7" s="9">
         <f>('Composite Stats'!$B7+'Composite Stats'!$C7)/2/$H7</f>
@@ -10555,17 +10560,17 @@
         <v>32.4</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="25">
+      <c r="B8" s="24">
         <v>1.5</v>
       </c>
       <c r="C8" s="8">
         <v>3</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="24">
         <v>2</v>
       </c>
       <c r="E8" s="8">
@@ -10584,12 +10589,12 @@
         <v>7</v>
       </c>
       <c r="I8" s="9">
-        <f>('Composite Stats'!$B8+'Composite Stats'!$C8)/2/$H8</f>
-        <v>81.428571428571431</v>
+        <f>('Composite Stats'!$B8+'Composite Stats'!$C8+'Base Stat Progression'!$B10+'Base Stat Progression'!$C10)/4/$H8</f>
+        <v>71.607142857142861</v>
       </c>
       <c r="J8" s="9">
-        <f>('Composite Stats'!$B8+'Composite Stats'!$C8)/2/$H8*1.5</f>
-        <v>122.14285714285714</v>
+        <f>('Composite Stats'!$B8+'Composite Stats'!$C8+'Base Stat Progression'!$B10+'Base Stat Progression'!$C10)/4/$H8*1.5</f>
+        <v>107.41071428571429</v>
       </c>
       <c r="K8" s="9">
         <f>('Composite Stats'!$B8+'Composite Stats'!$C8)/2/$H8</f>
@@ -10604,17 +10609,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="25">
+      <c r="B9" s="24">
         <v>1.5</v>
       </c>
       <c r="C9" s="8">
         <v>3</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="24">
         <v>2</v>
       </c>
       <c r="E9" s="8">
@@ -10633,12 +10638,12 @@
         <v>7</v>
       </c>
       <c r="I9" s="9">
-        <f>('Composite Stats'!$B9+'Composite Stats'!$C9)/2/$H9</f>
-        <v>90.571428571428569</v>
+        <f>('Composite Stats'!$B9+'Composite Stats'!$C9+'Base Stat Progression'!$B11+'Base Stat Progression'!$C11)/4/$H9</f>
+        <v>79.142857142857139</v>
       </c>
       <c r="J9" s="9">
-        <f>('Composite Stats'!$B9+'Composite Stats'!$C9)/2/$H9*1.5</f>
-        <v>135.85714285714286</v>
+        <f>('Composite Stats'!$B9+'Composite Stats'!$C9+'Base Stat Progression'!$B11+'Base Stat Progression'!$C11)/4/$H9*1.5</f>
+        <v>118.71428571428571</v>
       </c>
       <c r="K9" s="9">
         <f>('Composite Stats'!$B9+'Composite Stats'!$C9)/2/$H9</f>
@@ -10653,17 +10658,17 @@
         <v>33.6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="25">
+      <c r="B10" s="24">
         <v>1.5</v>
       </c>
       <c r="C10" s="8">
         <v>3</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="24">
         <v>2</v>
       </c>
       <c r="E10" s="8">
@@ -10682,12 +10687,12 @@
         <v>7</v>
       </c>
       <c r="I10" s="9">
-        <f>('Composite Stats'!$B10+'Composite Stats'!$C10)/2/$H10</f>
-        <v>99.714285714285708</v>
+        <f>('Composite Stats'!$B10+'Composite Stats'!$C10+'Base Stat Progression'!$B12+'Base Stat Progression'!$C12)/4/$H10</f>
+        <v>86.678571428571431</v>
       </c>
       <c r="J10" s="9">
-        <f>('Composite Stats'!$B10+'Composite Stats'!$C10)/2/$H10*1.5</f>
-        <v>149.57142857142856</v>
+        <f>('Composite Stats'!$B10+'Composite Stats'!$C10+'Base Stat Progression'!$B12+'Base Stat Progression'!$C12)/4/$H10*1.5</f>
+        <v>130.01785714285714</v>
       </c>
       <c r="K10" s="9">
         <f>('Composite Stats'!$B10+'Composite Stats'!$C10)/2/$H10</f>
@@ -10702,17 +10707,17 @@
         <v>34.200000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="24">
         <v>1.5</v>
       </c>
       <c r="C11" s="8">
         <v>3</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="24">
         <v>2</v>
       </c>
       <c r="E11" s="8">
@@ -10731,12 +10736,12 @@
         <v>7</v>
       </c>
       <c r="I11" s="9">
-        <f>('Composite Stats'!$B11+'Composite Stats'!$C11)/2/$H11</f>
-        <v>108.85714285714288</v>
+        <f>('Composite Stats'!$B11+'Composite Stats'!$C11+'Base Stat Progression'!$B13+'Base Stat Progression'!$C13)/4/$H11</f>
+        <v>94.214285714285737</v>
       </c>
       <c r="J11" s="9">
-        <f>('Composite Stats'!$B11+'Composite Stats'!$C11)/2/$H11*1.5</f>
-        <v>163.28571428571431</v>
+        <f>('Composite Stats'!$B11+'Composite Stats'!$C11+'Base Stat Progression'!$B13+'Base Stat Progression'!$C13)/4/$H11*1.5</f>
+        <v>141.32142857142861</v>
       </c>
       <c r="K11" s="9">
         <f>('Composite Stats'!$B11+'Composite Stats'!$C11)/2/$H11</f>
@@ -10751,17 +10756,17 @@
         <v>34.799999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="25">
         <v>1.5</v>
       </c>
       <c r="C12" s="8">
         <v>4</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="24">
         <v>2.5</v>
       </c>
       <c r="E12" s="8">
@@ -10780,12 +10785,12 @@
         <v>7</v>
       </c>
       <c r="I12" s="9">
-        <f>('Composite Stats'!$B12+'Composite Stats'!$C12)/2/$H12</f>
-        <v>118.00000000000001</v>
+        <f>('Composite Stats'!$B12+'Composite Stats'!$C12+'Base Stat Progression'!$B14+'Base Stat Progression'!$C14)/4/$H12</f>
+        <v>101.75000000000001</v>
       </c>
       <c r="J12" s="9">
-        <f>('Composite Stats'!$B12+'Composite Stats'!$C12)/2/$H12*1.5</f>
-        <v>177.00000000000003</v>
+        <f>('Composite Stats'!$B12+'Composite Stats'!$C12+'Base Stat Progression'!$B14+'Base Stat Progression'!$C14)/4/$H12*1.5</f>
+        <v>152.62500000000003</v>
       </c>
       <c r="K12" s="9">
         <f>('Composite Stats'!$B12+'Composite Stats'!$C12)/2/$H12</f>
@@ -10800,17 +10805,17 @@
         <v>35.4</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>11</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="25">
         <v>1.5</v>
       </c>
       <c r="C13" s="8">
         <v>4</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="24">
         <v>2.5</v>
       </c>
       <c r="E13" s="8">
@@ -10829,12 +10834,12 @@
         <v>7</v>
       </c>
       <c r="I13" s="9">
-        <f>('Composite Stats'!$B13+'Composite Stats'!$C13)/2/$H13</f>
-        <v>127.14285714285718</v>
+        <f>('Composite Stats'!$B13+'Composite Stats'!$C13+'Base Stat Progression'!$B15+'Base Stat Progression'!$C15)/4/$H13</f>
+        <v>109.28571428571432</v>
       </c>
       <c r="J13" s="9">
-        <f>('Composite Stats'!$B13+'Composite Stats'!$C13)/2/$H13*1.5</f>
-        <v>190.71428571428578</v>
+        <f>('Composite Stats'!$B13+'Composite Stats'!$C13+'Base Stat Progression'!$B15+'Base Stat Progression'!$C15)/4/$H13*1.5</f>
+        <v>163.92857142857147</v>
       </c>
       <c r="K13" s="9">
         <f>('Composite Stats'!$B13+'Composite Stats'!$C13)/2/$H13</f>
@@ -10849,17 +10854,17 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>12</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="25">
         <v>1.5</v>
       </c>
       <c r="C14" s="8">
         <v>4</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="24">
         <v>2.5</v>
       </c>
       <c r="E14" s="8">
@@ -10878,12 +10883,12 @@
         <v>7</v>
       </c>
       <c r="I14" s="9">
-        <f>('Composite Stats'!$B14+'Composite Stats'!$C14)/2/$H14</f>
-        <v>136.28571428571431</v>
+        <f>('Composite Stats'!$B14+'Composite Stats'!$C14+'Base Stat Progression'!$B16+'Base Stat Progression'!$C16)/4/$H14</f>
+        <v>116.82142857142858</v>
       </c>
       <c r="J14" s="9">
-        <f>('Composite Stats'!$B14+'Composite Stats'!$C14)/2/$H14*1.5</f>
-        <v>204.42857142857144</v>
+        <f>('Composite Stats'!$B14+'Composite Stats'!$C14+'Base Stat Progression'!$B16+'Base Stat Progression'!$C16)/4/$H14*1.5</f>
+        <v>175.23214285714289</v>
       </c>
       <c r="K14" s="9">
         <f>('Composite Stats'!$B14+'Composite Stats'!$C14)/2/$H14</f>
@@ -10898,17 +10903,17 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <v>13</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="25">
         <v>1.5</v>
       </c>
       <c r="C15" s="8">
         <v>4</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="24">
         <v>2.5</v>
       </c>
       <c r="E15" s="8">
@@ -10927,12 +10932,12 @@
         <v>7</v>
       </c>
       <c r="I15" s="9">
-        <f>('Composite Stats'!$B15+'Composite Stats'!$C15)/2/$H15</f>
-        <v>145.42857142857147</v>
+        <f>('Composite Stats'!$B15+'Composite Stats'!$C15+'Base Stat Progression'!$B17+'Base Stat Progression'!$C17)/4/$H15</f>
+        <v>124.35714285714289</v>
       </c>
       <c r="J15" s="9">
-        <f>('Composite Stats'!$B15+'Composite Stats'!$C15)/2/$H15*1.5</f>
-        <v>218.14285714285722</v>
+        <f>('Composite Stats'!$B15+'Composite Stats'!$C15+'Base Stat Progression'!$B17+'Base Stat Progression'!$C17)/4/$H15*1.5</f>
+        <v>186.53571428571433</v>
       </c>
       <c r="K15" s="9">
         <f>('Composite Stats'!$B15+'Composite Stats'!$C15)/2/$H15</f>
@@ -10947,17 +10952,17 @@
         <v>37.199999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10">
         <v>14</v>
       </c>
-      <c r="B16" s="26">
+      <c r="B16" s="25">
         <v>1.5</v>
       </c>
       <c r="C16" s="8">
         <v>4</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="24">
         <v>2.5</v>
       </c>
       <c r="E16" s="8">
@@ -10976,12 +10981,12 @@
         <v>7</v>
       </c>
       <c r="I16" s="9">
-        <f>('Composite Stats'!$B16+'Composite Stats'!$C16)/2/$H16</f>
-        <v>154.57142857142858</v>
+        <f>('Composite Stats'!$B16+'Composite Stats'!$C16+'Base Stat Progression'!$B18+'Base Stat Progression'!$C18)/4/$H16</f>
+        <v>131.89285714285717</v>
       </c>
       <c r="J16" s="9">
-        <f>('Composite Stats'!$B16+'Composite Stats'!$C16)/2/$H16*1.5</f>
-        <v>231.85714285714289</v>
+        <f>('Composite Stats'!$B16+'Composite Stats'!$C16+'Base Stat Progression'!$B18+'Base Stat Progression'!$C18)/4/$H16*1.5</f>
+        <v>197.83928571428575</v>
       </c>
       <c r="K16" s="9">
         <f>('Composite Stats'!$B16+'Composite Stats'!$C16)/2/$H16</f>
@@ -10996,17 +11001,17 @@
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10">
         <v>15</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="25">
         <v>2</v>
       </c>
       <c r="C17" s="8">
         <v>4</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="24">
         <v>2.5</v>
       </c>
       <c r="E17" s="8">
@@ -11025,12 +11030,12 @@
         <v>7</v>
       </c>
       <c r="I17" s="9">
-        <f>('Composite Stats'!$B17+'Composite Stats'!$C17)/2/$H17</f>
-        <v>163.71428571428575</v>
+        <f>('Composite Stats'!$B17+'Composite Stats'!$C17+'Base Stat Progression'!$B19+'Base Stat Progression'!$C19)/4/$H17</f>
+        <v>139.42857142857147</v>
       </c>
       <c r="J17" s="9">
-        <f>('Composite Stats'!$B17+'Composite Stats'!$C17)/2/$H17*1.5</f>
-        <v>245.57142857142861</v>
+        <f>('Composite Stats'!$B17+'Composite Stats'!$C17+'Base Stat Progression'!$B19+'Base Stat Progression'!$C19)/4/$H17*1.5</f>
+        <v>209.14285714285722</v>
       </c>
       <c r="K17" s="9">
         <f>('Composite Stats'!$B17+'Composite Stats'!$C17)/2/$H17</f>
@@ -11045,17 +11050,17 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
         <v>16</v>
       </c>
-      <c r="B18" s="26">
+      <c r="B18" s="25">
         <v>2</v>
       </c>
       <c r="C18" s="8">
         <v>4</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="24">
         <v>2.5</v>
       </c>
       <c r="E18" s="8">
@@ -11074,12 +11079,12 @@
         <v>7</v>
       </c>
       <c r="I18" s="9">
-        <f>('Composite Stats'!$B18+'Composite Stats'!$C18)/2/$H18</f>
-        <v>172.85714285714286</v>
+        <f>('Composite Stats'!$B18+'Composite Stats'!$C18+'Base Stat Progression'!$B20+'Base Stat Progression'!$C20)/4/$H18</f>
+        <v>146.96428571428572</v>
       </c>
       <c r="J18" s="9">
-        <f>('Composite Stats'!$B18+'Composite Stats'!$C18)/2/$H18*1.5</f>
-        <v>259.28571428571428</v>
+        <f>('Composite Stats'!$B18+'Composite Stats'!$C18+'Base Stat Progression'!$B20+'Base Stat Progression'!$C20)/4/$H18*1.5</f>
+        <v>220.44642857142858</v>
       </c>
       <c r="K18" s="9">
         <f>('Composite Stats'!$B18+'Composite Stats'!$C18)/2/$H18</f>
@@ -11094,17 +11099,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>17</v>
       </c>
-      <c r="B19" s="26">
+      <c r="B19" s="25">
         <v>2</v>
       </c>
       <c r="C19" s="8">
         <v>4</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="24">
         <v>2.5</v>
       </c>
       <c r="E19" s="8">
@@ -11123,12 +11128,12 @@
         <v>7</v>
       </c>
       <c r="I19" s="9">
-        <f>('Composite Stats'!$B19+'Composite Stats'!$C19)/2/$H19</f>
-        <v>182</v>
+        <f>('Composite Stats'!$B19+'Composite Stats'!$C19+'Base Stat Progression'!$B21+'Base Stat Progression'!$C21)/4/$H19</f>
+        <v>154.50000000000003</v>
       </c>
       <c r="J19" s="9">
-        <f>('Composite Stats'!$B19+'Composite Stats'!$C19)/2/$H19*1.5</f>
-        <v>273</v>
+        <f>('Composite Stats'!$B19+'Composite Stats'!$C19+'Base Stat Progression'!$B21+'Base Stat Progression'!$C21)/4/$H19*1.5</f>
+        <v>231.75000000000006</v>
       </c>
       <c r="K19" s="9">
         <f>('Composite Stats'!$B19+'Composite Stats'!$C19)/2/$H19</f>
@@ -11143,17 +11148,17 @@
         <v>39.599999999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10">
         <v>18</v>
       </c>
-      <c r="B20" s="26">
+      <c r="B20" s="25">
         <v>2</v>
       </c>
       <c r="C20" s="8">
         <v>4</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="24">
         <v>2.5</v>
       </c>
       <c r="E20" s="8">
@@ -11172,12 +11177,12 @@
         <v>7</v>
       </c>
       <c r="I20" s="9">
-        <f>('Composite Stats'!$B20+'Composite Stats'!$C20)/2/$H20</f>
-        <v>191.14285714285714</v>
+        <f>('Composite Stats'!$B20+'Composite Stats'!$C20+'Base Stat Progression'!$B22+'Base Stat Progression'!$C22)/4/$H20</f>
+        <v>162.03571428571428</v>
       </c>
       <c r="J20" s="9">
-        <f>('Composite Stats'!$B20+'Composite Stats'!$C20)/2/$H20*1.5</f>
-        <v>286.71428571428572</v>
+        <f>('Composite Stats'!$B20+'Composite Stats'!$C20+'Base Stat Progression'!$B22+'Base Stat Progression'!$C22)/4/$H20*1.5</f>
+        <v>243.05357142857142</v>
       </c>
       <c r="K20" s="9">
         <f>('Composite Stats'!$B20+'Composite Stats'!$C20)/2/$H20</f>
@@ -11192,17 +11197,17 @@
         <v>40.199999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <v>19</v>
       </c>
-      <c r="B21" s="26">
+      <c r="B21" s="25">
         <v>2</v>
       </c>
       <c r="C21" s="8">
         <v>4</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="24">
         <v>2.5</v>
       </c>
       <c r="E21" s="8">
@@ -11221,12 +11226,12 @@
         <v>7</v>
       </c>
       <c r="I21" s="9">
-        <f>('Composite Stats'!$B21+'Composite Stats'!$C21)/2/$H21</f>
-        <v>200.28571428571428</v>
+        <f>('Composite Stats'!$B21+'Composite Stats'!$C21+'Base Stat Progression'!$B23+'Base Stat Progression'!$C23)/4/$H21</f>
+        <v>169.57142857142858</v>
       </c>
       <c r="J21" s="9">
-        <f>('Composite Stats'!$B21+'Composite Stats'!$C21)/2/$H21*1.5</f>
-        <v>300.42857142857144</v>
+        <f>('Composite Stats'!$B21+'Composite Stats'!$C21+'Base Stat Progression'!$B23+'Base Stat Progression'!$C23)/4/$H21*1.5</f>
+        <v>254.35714285714289</v>
       </c>
       <c r="K21" s="9">
         <f>('Composite Stats'!$B21+'Composite Stats'!$C21)/2/$H21</f>
@@ -11241,17 +11246,17 @@
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>20</v>
       </c>
-      <c r="B22" s="26">
+      <c r="B22" s="25">
         <v>2</v>
       </c>
       <c r="C22" s="8">
         <v>5</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="25">
         <v>3</v>
       </c>
       <c r="E22" s="8">
@@ -11270,12 +11275,12 @@
         <v>6</v>
       </c>
       <c r="I22" s="9">
-        <f>('Composite Stats'!$B22+'Composite Stats'!$C22)/2/$H22</f>
-        <v>244.33333333333337</v>
+        <f>('Composite Stats'!$B22+'Composite Stats'!$C22+'Base Stat Progression'!$B24+'Base Stat Progression'!$C24)/4/$H22</f>
+        <v>206.62500000000003</v>
       </c>
       <c r="J22" s="9">
-        <f>('Composite Stats'!$B22+'Composite Stats'!$C22)/2/$H22*1.5</f>
-        <v>366.50000000000006</v>
+        <f>('Composite Stats'!$B22+'Composite Stats'!$C22+'Base Stat Progression'!$B24+'Base Stat Progression'!$C24)/4/$H22*1.5</f>
+        <v>309.93750000000006</v>
       </c>
       <c r="K22" s="9">
         <f>('Composite Stats'!$B22+'Composite Stats'!$C22)/2/$H22</f>
@@ -11290,17 +11295,17 @@
         <v>41.4</v>
       </c>
     </row>
-    <row r="23" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10">
         <v>21</v>
       </c>
-      <c r="B23" s="26">
+      <c r="B23" s="25">
         <v>2</v>
       </c>
       <c r="C23" s="8">
         <v>5</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="25">
         <v>3</v>
       </c>
       <c r="E23" s="8">
@@ -11319,12 +11324,12 @@
         <v>6</v>
       </c>
       <c r="I23" s="9">
-        <f>('Composite Stats'!$B23+'Composite Stats'!$C23)/2/$H23</f>
-        <v>255</v>
+        <f>('Composite Stats'!$B23+'Composite Stats'!$C23+'Base Stat Progression'!$B25+'Base Stat Progression'!$C25)/4/$H23</f>
+        <v>215.41666666666671</v>
       </c>
       <c r="J23" s="9">
-        <f>('Composite Stats'!$B23+'Composite Stats'!$C23)/2/$H23*1.5</f>
-        <v>382.5</v>
+        <f>('Composite Stats'!$B23+'Composite Stats'!$C23+'Base Stat Progression'!$B25+'Base Stat Progression'!$C25)/4/$H23*1.5</f>
+        <v>323.12500000000006</v>
       </c>
       <c r="K23" s="9">
         <f>('Composite Stats'!$B23+'Composite Stats'!$C23)/2/$H23</f>
@@ -11343,17 +11348,17 @@
         <v>14.333333333333334</v>
       </c>
     </row>
-    <row r="24" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>22</v>
       </c>
-      <c r="B24" s="26">
+      <c r="B24" s="25">
         <v>2</v>
       </c>
       <c r="C24" s="8">
         <v>5</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="25">
         <v>3</v>
       </c>
       <c r="E24" s="8">
@@ -11372,12 +11377,12 @@
         <v>6</v>
       </c>
       <c r="I24" s="9">
-        <f>('Composite Stats'!$B24+'Composite Stats'!$C24)/2/$H24</f>
-        <v>265.66666666666669</v>
+        <f>('Composite Stats'!$B24+'Composite Stats'!$C24+'Base Stat Progression'!$B26+'Base Stat Progression'!$C26)/4/$H24</f>
+        <v>224.20833333333334</v>
       </c>
       <c r="J24" s="9">
-        <f>('Composite Stats'!$B24+'Composite Stats'!$C24)/2/$H24*1.5</f>
-        <v>398.5</v>
+        <f>('Composite Stats'!$B24+'Composite Stats'!$C24+'Base Stat Progression'!$B26+'Base Stat Progression'!$C26)/4/$H24*1.5</f>
+        <v>336.3125</v>
       </c>
       <c r="K24" s="9">
         <f>('Composite Stats'!$B24+'Composite Stats'!$C24)/2/$H24</f>
@@ -11392,17 +11397,17 @@
         <v>42.599999999999994</v>
       </c>
     </row>
-    <row r="25" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10">
         <v>23</v>
       </c>
-      <c r="B25" s="26">
+      <c r="B25" s="25">
         <v>2</v>
       </c>
       <c r="C25" s="8">
         <v>5</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="25">
         <v>3</v>
       </c>
       <c r="E25" s="8">
@@ -11421,12 +11426,12 @@
         <v>6</v>
       </c>
       <c r="I25" s="9">
-        <f>('Composite Stats'!$B25+'Composite Stats'!$C25)/2/$H25</f>
-        <v>276.33333333333337</v>
+        <f>('Composite Stats'!$B25+'Composite Stats'!$C25+'Base Stat Progression'!$B27+'Base Stat Progression'!$C27)/4/$H25</f>
+        <v>233.00000000000003</v>
       </c>
       <c r="J25" s="9">
-        <f>('Composite Stats'!$B25+'Composite Stats'!$C25)/2/$H25*1.5</f>
-        <v>414.50000000000006</v>
+        <f>('Composite Stats'!$B25+'Composite Stats'!$C25+'Base Stat Progression'!$B27+'Base Stat Progression'!$C27)/4/$H25*1.5</f>
+        <v>349.50000000000006</v>
       </c>
       <c r="K25" s="9">
         <f>('Composite Stats'!$B25+'Composite Stats'!$C25)/2/$H25</f>
@@ -11441,17 +11446,17 @@
         <v>43.199999999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10">
         <v>24</v>
       </c>
-      <c r="B26" s="26">
+      <c r="B26" s="25">
         <v>2</v>
       </c>
       <c r="C26" s="8">
         <v>5</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="25">
         <v>3</v>
       </c>
       <c r="E26" s="8">
@@ -11470,12 +11475,12 @@
         <v>6</v>
       </c>
       <c r="I26" s="9">
-        <f>('Composite Stats'!$B26+'Composite Stats'!$C26)/2/$H26</f>
-        <v>287.00000000000006</v>
+        <f>('Composite Stats'!$B26+'Composite Stats'!$C26+'Base Stat Progression'!$B28+'Base Stat Progression'!$C28)/4/$H26</f>
+        <v>241.79166666666666</v>
       </c>
       <c r="J26" s="9">
-        <f>('Composite Stats'!$B26+'Composite Stats'!$C26)/2/$H26*1.5</f>
-        <v>430.50000000000011</v>
+        <f>('Composite Stats'!$B26+'Composite Stats'!$C26+'Base Stat Progression'!$B28+'Base Stat Progression'!$C28)/4/$H26*1.5</f>
+        <v>362.6875</v>
       </c>
       <c r="K26" s="9">
         <f>('Composite Stats'!$B26+'Composite Stats'!$C26)/2/$H26</f>
@@ -11490,17 +11495,17 @@
         <v>43.8</v>
       </c>
     </row>
-    <row r="27" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <v>25</v>
       </c>
-      <c r="B27" s="26">
+      <c r="B27" s="25">
         <v>2.5</v>
       </c>
       <c r="C27" s="8">
         <v>5</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="25">
         <v>3</v>
       </c>
       <c r="E27" s="8">
@@ -11519,12 +11524,12 @@
         <v>6</v>
       </c>
       <c r="I27" s="9">
-        <f>('Composite Stats'!$B27+'Composite Stats'!$C27)/2/$H27</f>
-        <v>297.66666666666669</v>
+        <f>('Composite Stats'!$B27+'Composite Stats'!$C27+'Base Stat Progression'!$B29+'Base Stat Progression'!$C29)/4/$H27</f>
+        <v>250.58333333333337</v>
       </c>
       <c r="J27" s="9">
-        <f>('Composite Stats'!$B27+'Composite Stats'!$C27)/2/$H27*1.5</f>
-        <v>446.5</v>
+        <f>('Composite Stats'!$B27+'Composite Stats'!$C27+'Base Stat Progression'!$B29+'Base Stat Progression'!$C29)/4/$H27*1.5</f>
+        <v>375.87500000000006</v>
       </c>
       <c r="K27" s="9">
         <f>('Composite Stats'!$B27+'Composite Stats'!$C27)/2/$H27</f>
@@ -11539,17 +11544,17 @@
         <v>44.399999999999991</v>
       </c>
     </row>
-    <row r="28" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10">
         <v>26</v>
       </c>
-      <c r="B28" s="26">
+      <c r="B28" s="25">
         <v>2.5</v>
       </c>
       <c r="C28" s="8">
         <v>5</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="25">
         <v>3</v>
       </c>
       <c r="E28" s="8">
@@ -11568,12 +11573,12 @@
         <v>6</v>
       </c>
       <c r="I28" s="9">
-        <f>('Composite Stats'!$B28+'Composite Stats'!$C28)/2/$H28</f>
-        <v>308.33333333333331</v>
+        <f>('Composite Stats'!$B28+'Composite Stats'!$C28+'Base Stat Progression'!$B30+'Base Stat Progression'!$C30)/4/$H28</f>
+        <v>259.37500000000006</v>
       </c>
       <c r="J28" s="9">
-        <f>('Composite Stats'!$B28+'Composite Stats'!$C28)/2/$H28*1.5</f>
-        <v>462.5</v>
+        <f>('Composite Stats'!$B28+'Composite Stats'!$C28+'Base Stat Progression'!$B30+'Base Stat Progression'!$C30)/4/$H28*1.5</f>
+        <v>389.06250000000011</v>
       </c>
       <c r="K28" s="9">
         <f>('Composite Stats'!$B28+'Composite Stats'!$C28)/2/$H28</f>
@@ -11588,17 +11593,17 @@
         <v>44.999999999999993</v>
       </c>
     </row>
-    <row r="29" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>27</v>
       </c>
-      <c r="B29" s="26">
+      <c r="B29" s="25">
         <v>2.5</v>
       </c>
       <c r="C29" s="8">
         <v>5</v>
       </c>
-      <c r="D29" s="26">
+      <c r="D29" s="25">
         <v>3</v>
       </c>
       <c r="E29" s="8">
@@ -11617,12 +11622,12 @@
         <v>6</v>
       </c>
       <c r="I29" s="9">
-        <f>('Composite Stats'!$B29+'Composite Stats'!$C29)/2/$H29</f>
-        <v>319</v>
+        <f>('Composite Stats'!$B29+'Composite Stats'!$C29+'Base Stat Progression'!$B31+'Base Stat Progression'!$C31)/4/$H29</f>
+        <v>268.16666666666669</v>
       </c>
       <c r="J29" s="9">
-        <f>('Composite Stats'!$B29+'Composite Stats'!$C29)/2/$H29*1.5</f>
-        <v>478.5</v>
+        <f>('Composite Stats'!$B29+'Composite Stats'!$C29+'Base Stat Progression'!$B31+'Base Stat Progression'!$C31)/4/$H29*1.5</f>
+        <v>402.25</v>
       </c>
       <c r="K29" s="9">
         <f>('Composite Stats'!$B29+'Composite Stats'!$C29)/2/$H29</f>
@@ -11637,17 +11642,17 @@
         <v>45.599999999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <v>28</v>
       </c>
-      <c r="B30" s="26">
+      <c r="B30" s="25">
         <v>2.5</v>
       </c>
       <c r="C30" s="8">
         <v>5</v>
       </c>
-      <c r="D30" s="26">
+      <c r="D30" s="25">
         <v>3</v>
       </c>
       <c r="E30" s="8">
@@ -11666,12 +11671,12 @@
         <v>6</v>
       </c>
       <c r="I30" s="9">
-        <f>('Composite Stats'!$B30+'Composite Stats'!$C30)/2/$H30</f>
-        <v>329.66666666666669</v>
+        <f>('Composite Stats'!$B30+'Composite Stats'!$C30+'Base Stat Progression'!$B32+'Base Stat Progression'!$C32)/4/$H30</f>
+        <v>276.95833333333343</v>
       </c>
       <c r="J30" s="9">
-        <f>('Composite Stats'!$B30+'Composite Stats'!$C30)/2/$H30*1.5</f>
-        <v>494.5</v>
+        <f>('Composite Stats'!$B30+'Composite Stats'!$C30+'Base Stat Progression'!$B32+'Base Stat Progression'!$C32)/4/$H30*1.5</f>
+        <v>415.43750000000011</v>
       </c>
       <c r="K30" s="9">
         <f>('Composite Stats'!$B30+'Composite Stats'!$C30)/2/$H30</f>
@@ -11686,17 +11691,17 @@
         <v>46.199999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10">
         <v>29</v>
       </c>
-      <c r="B31" s="26">
+      <c r="B31" s="25">
         <v>2.5</v>
       </c>
       <c r="C31" s="8">
         <v>5</v>
       </c>
-      <c r="D31" s="26">
+      <c r="D31" s="25">
         <v>3</v>
       </c>
       <c r="E31" s="8">
@@ -11715,12 +11720,12 @@
         <v>6</v>
       </c>
       <c r="I31" s="9">
-        <f>('Composite Stats'!$B31+'Composite Stats'!$C31)/2/$H31</f>
-        <v>340.33333333333331</v>
+        <f>('Composite Stats'!$B31+'Composite Stats'!$C31+'Base Stat Progression'!$B33+'Base Stat Progression'!$C33)/4/$H31</f>
+        <v>285.75000000000006</v>
       </c>
       <c r="J31" s="9">
-        <f>('Composite Stats'!$B31+'Composite Stats'!$C31)/2/$H31*1.5</f>
-        <v>510.5</v>
+        <f>('Composite Stats'!$B31+'Composite Stats'!$C31+'Base Stat Progression'!$B33+'Base Stat Progression'!$C33)/4/$H31*1.5</f>
+        <v>428.62500000000011</v>
       </c>
       <c r="K31" s="9">
         <f>('Composite Stats'!$B31+'Composite Stats'!$C31)/2/$H31</f>
@@ -11735,17 +11740,17 @@
         <v>46.8</v>
       </c>
     </row>
-    <row r="32" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>30</v>
       </c>
-      <c r="B32" s="26">
+      <c r="B32" s="25">
         <v>2.5</v>
       </c>
       <c r="C32" s="4">
         <v>5</v>
       </c>
-      <c r="D32" s="26">
+      <c r="D32" s="25">
         <v>3.5</v>
       </c>
       <c r="E32" s="8">
@@ -11764,12 +11769,12 @@
         <v>6</v>
       </c>
       <c r="I32" s="9">
-        <f>('Composite Stats'!$B32+'Composite Stats'!$C32)/2/$H32</f>
-        <v>351</v>
+        <f>('Composite Stats'!$B32+'Composite Stats'!$C32+'Base Stat Progression'!$B34+'Base Stat Progression'!$C34)/4/$H32</f>
+        <v>294.54166666666669</v>
       </c>
       <c r="J32" s="9">
-        <f>('Composite Stats'!$B32+'Composite Stats'!$C32)/2/$H32*1.5</f>
-        <v>526.5</v>
+        <f>('Composite Stats'!$B32+'Composite Stats'!$C32+'Base Stat Progression'!$B34+'Base Stat Progression'!$C34)/4/$H32*1.5</f>
+        <v>441.8125</v>
       </c>
       <c r="K32" s="9">
         <f>('Composite Stats'!$B32+'Composite Stats'!$C32)/2/$H32</f>
@@ -11784,17 +11789,17 @@
         <v>47.4</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <v>31</v>
       </c>
-      <c r="B33" s="26">
+      <c r="B33" s="25">
         <v>2.5</v>
       </c>
       <c r="C33" s="4">
         <v>5</v>
       </c>
-      <c r="D33" s="26">
+      <c r="D33" s="25">
         <v>3.5</v>
       </c>
       <c r="E33" s="8">
@@ -11813,12 +11818,12 @@
         <v>6</v>
       </c>
       <c r="I33" s="9">
-        <f>('Composite Stats'!$B33+'Composite Stats'!$C33)/2/$H33</f>
-        <v>361.66666666666669</v>
+        <f>('Composite Stats'!$B33+'Composite Stats'!$C33+'Base Stat Progression'!$B35+'Base Stat Progression'!$C35)/4/$H33</f>
+        <v>303.33333333333331</v>
       </c>
       <c r="J33" s="9">
-        <f>('Composite Stats'!$B33+'Composite Stats'!$C33)/2/$H33*1.5</f>
-        <v>542.5</v>
+        <f>('Composite Stats'!$B33+'Composite Stats'!$C33+'Base Stat Progression'!$B35+'Base Stat Progression'!$C35)/4/$H33*1.5</f>
+        <v>455</v>
       </c>
       <c r="K33" s="9">
         <f>('Composite Stats'!$B33+'Composite Stats'!$C33)/2/$H33</f>
@@ -11833,17 +11838,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10">
         <v>32</v>
       </c>
-      <c r="B34" s="26">
+      <c r="B34" s="25">
         <v>2.5</v>
       </c>
       <c r="C34" s="4">
         <v>5</v>
       </c>
-      <c r="D34" s="26">
+      <c r="D34" s="25">
         <v>3.5</v>
       </c>
       <c r="E34" s="8">
@@ -11862,12 +11867,12 @@
         <v>6</v>
       </c>
       <c r="I34" s="9">
-        <f>('Composite Stats'!$B34+'Composite Stats'!$C34)/2/$H34</f>
-        <v>372.33333333333331</v>
+        <f>('Composite Stats'!$B34+'Composite Stats'!$C34+'Base Stat Progression'!$B36+'Base Stat Progression'!$C36)/4/$H34</f>
+        <v>312.125</v>
       </c>
       <c r="J34" s="9">
-        <f>('Composite Stats'!$B34+'Composite Stats'!$C34)/2/$H34*1.5</f>
-        <v>558.5</v>
+        <f>('Composite Stats'!$B34+'Composite Stats'!$C34+'Base Stat Progression'!$B36+'Base Stat Progression'!$C36)/4/$H34*1.5</f>
+        <v>468.1875</v>
       </c>
       <c r="K34" s="9">
         <f>('Composite Stats'!$B34+'Composite Stats'!$C34)/2/$H34</f>
@@ -11882,17 +11887,17 @@
         <v>48.6</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10">
         <v>33</v>
       </c>
-      <c r="B35" s="26">
+      <c r="B35" s="25">
         <v>2.5</v>
       </c>
       <c r="C35" s="4">
         <v>5</v>
       </c>
-      <c r="D35" s="26">
+      <c r="D35" s="25">
         <v>3.5</v>
       </c>
       <c r="E35" s="8">
@@ -11911,12 +11916,12 @@
         <v>6</v>
       </c>
       <c r="I35" s="9">
-        <f>('Composite Stats'!$B35+'Composite Stats'!$C35)/2/$H35</f>
-        <v>383</v>
+        <f>('Composite Stats'!$B35+'Composite Stats'!$C35+'Base Stat Progression'!$B37+'Base Stat Progression'!$C37)/4/$H35</f>
+        <v>320.91666666666669</v>
       </c>
       <c r="J35" s="9">
-        <f>('Composite Stats'!$B35+'Composite Stats'!$C35)/2/$H35*1.5</f>
-        <v>574.5</v>
+        <f>('Composite Stats'!$B35+'Composite Stats'!$C35+'Base Stat Progression'!$B37+'Base Stat Progression'!$C37)/4/$H35*1.5</f>
+        <v>481.375</v>
       </c>
       <c r="K35" s="9">
         <f>('Composite Stats'!$B35+'Composite Stats'!$C35)/2/$H35</f>
@@ -11931,17 +11936,17 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10">
         <v>34</v>
       </c>
-      <c r="B36" s="26">
+      <c r="B36" s="25">
         <v>2.5</v>
       </c>
       <c r="C36" s="4">
         <v>5</v>
       </c>
-      <c r="D36" s="26">
+      <c r="D36" s="25">
         <v>3.5</v>
       </c>
       <c r="E36" s="8">
@@ -11960,12 +11965,12 @@
         <v>6</v>
       </c>
       <c r="I36" s="9">
-        <f>('Composite Stats'!$B36+'Composite Stats'!$C36)/2/$H36</f>
-        <v>393.66666666666669</v>
+        <f>('Composite Stats'!$B36+'Composite Stats'!$C36+'Base Stat Progression'!$B38+'Base Stat Progression'!$C38)/4/$H36</f>
+        <v>329.70833333333337</v>
       </c>
       <c r="J36" s="9">
-        <f>('Composite Stats'!$B36+'Composite Stats'!$C36)/2/$H36*1.5</f>
-        <v>590.5</v>
+        <f>('Composite Stats'!$B36+'Composite Stats'!$C36+'Base Stat Progression'!$B38+'Base Stat Progression'!$C38)/4/$H36*1.5</f>
+        <v>494.56250000000006</v>
       </c>
       <c r="K36" s="9">
         <f>('Composite Stats'!$B36+'Composite Stats'!$C36)/2/$H36</f>
@@ -11980,17 +11985,17 @@
         <v>49.800000000000004</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10">
         <v>35</v>
       </c>
-      <c r="B37" s="26">
+      <c r="B37" s="25">
         <v>3</v>
       </c>
       <c r="C37" s="4">
         <v>5</v>
       </c>
-      <c r="D37" s="26">
+      <c r="D37" s="25">
         <v>3.5</v>
       </c>
       <c r="E37" s="8">
@@ -12009,12 +12014,12 @@
         <v>5</v>
       </c>
       <c r="I37" s="9">
-        <f>('Composite Stats'!$B37+'Composite Stats'!$C37)/2/$H37</f>
-        <v>485.2</v>
+        <f>('Composite Stats'!$B37+'Composite Stats'!$C37+'Base Stat Progression'!$B39+'Base Stat Progression'!$C39)/4/$H37</f>
+        <v>406.2</v>
       </c>
       <c r="J37" s="9">
-        <f>('Composite Stats'!$B37+'Composite Stats'!$C37)/2/$H37*1.5</f>
-        <v>727.8</v>
+        <f>('Composite Stats'!$B37+'Composite Stats'!$C37+'Base Stat Progression'!$B39+'Base Stat Progression'!$C39)/4/$H37*1.5</f>
+        <v>609.29999999999995</v>
       </c>
       <c r="K37" s="9">
         <f>('Composite Stats'!$B37+'Composite Stats'!$C37)/2/$H37</f>
@@ -12029,17 +12034,17 @@
         <v>50.400000000000006</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10">
         <v>36</v>
       </c>
-      <c r="B38" s="26">
+      <c r="B38" s="25">
         <v>3</v>
       </c>
       <c r="C38" s="4">
         <v>5</v>
       </c>
-      <c r="D38" s="26">
+      <c r="D38" s="25">
         <v>3.5</v>
       </c>
       <c r="E38" s="8">
@@ -12058,12 +12063,12 @@
         <v>5</v>
       </c>
       <c r="I38" s="9">
-        <f>('Composite Stats'!$B38+'Composite Stats'!$C38)/2/$H38</f>
-        <v>498</v>
+        <f>('Composite Stats'!$B38+'Composite Stats'!$C38+'Base Stat Progression'!$B40+'Base Stat Progression'!$C40)/4/$H38</f>
+        <v>416.75</v>
       </c>
       <c r="J38" s="9">
-        <f>('Composite Stats'!$B38+'Composite Stats'!$C38)/2/$H38*1.5</f>
-        <v>747</v>
+        <f>('Composite Stats'!$B38+'Composite Stats'!$C38+'Base Stat Progression'!$B40+'Base Stat Progression'!$C40)/4/$H38*1.5</f>
+        <v>625.125</v>
       </c>
       <c r="K38" s="9">
         <f>('Composite Stats'!$B38+'Composite Stats'!$C38)/2/$H38</f>
@@ -12078,17 +12083,17 @@
         <v>51.000000000000007</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10">
         <v>37</v>
       </c>
-      <c r="B39" s="26">
+      <c r="B39" s="25">
         <v>3</v>
       </c>
       <c r="C39" s="4">
         <v>5</v>
       </c>
-      <c r="D39" s="26">
+      <c r="D39" s="25">
         <v>3.5</v>
       </c>
       <c r="E39" s="8">
@@ -12107,12 +12112,12 @@
         <v>5</v>
       </c>
       <c r="I39" s="9">
-        <f>('Composite Stats'!$B39+'Composite Stats'!$C39)/2/$H39</f>
-        <v>510.8</v>
+        <f>('Composite Stats'!$B39+'Composite Stats'!$C39+'Base Stat Progression'!$B41+'Base Stat Progression'!$C41)/4/$H39</f>
+        <v>427.3</v>
       </c>
       <c r="J39" s="9">
-        <f>('Composite Stats'!$B39+'Composite Stats'!$C39)/2/$H39*1.5</f>
-        <v>766.2</v>
+        <f>('Composite Stats'!$B39+'Composite Stats'!$C39+'Base Stat Progression'!$B41+'Base Stat Progression'!$C41)/4/$H39*1.5</f>
+        <v>640.95000000000005</v>
       </c>
       <c r="K39" s="9">
         <f>('Composite Stats'!$B39+'Composite Stats'!$C39)/2/$H39</f>
@@ -12127,17 +12132,17 @@
         <v>51.600000000000009</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10">
         <v>38</v>
       </c>
-      <c r="B40" s="26">
+      <c r="B40" s="25">
         <v>3</v>
       </c>
       <c r="C40" s="4">
         <v>5</v>
       </c>
-      <c r="D40" s="26">
+      <c r="D40" s="25">
         <v>3.5</v>
       </c>
       <c r="E40" s="8">
@@ -12156,12 +12161,12 @@
         <v>5</v>
       </c>
       <c r="I40" s="9">
-        <f>('Composite Stats'!$B40+'Composite Stats'!$C40)/2/$H40</f>
-        <v>523.6</v>
+        <f>('Composite Stats'!$B40+'Composite Stats'!$C40+'Base Stat Progression'!$B42+'Base Stat Progression'!$C42)/4/$H40</f>
+        <v>437.85</v>
       </c>
       <c r="J40" s="9">
-        <f>('Composite Stats'!$B40+'Composite Stats'!$C40)/2/$H40*1.5</f>
-        <v>785.40000000000009</v>
+        <f>('Composite Stats'!$B40+'Composite Stats'!$C40+'Base Stat Progression'!$B42+'Base Stat Progression'!$C42)/4/$H40*1.5</f>
+        <v>656.77500000000009</v>
       </c>
       <c r="K40" s="9">
         <f>('Composite Stats'!$B40+'Composite Stats'!$C40)/2/$H40</f>
@@ -12176,17 +12181,17 @@
         <v>52.20000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10">
         <v>39</v>
       </c>
-      <c r="B41" s="26">
+      <c r="B41" s="25">
         <v>3</v>
       </c>
       <c r="C41" s="4">
         <v>5</v>
       </c>
-      <c r="D41" s="26">
+      <c r="D41" s="25">
         <v>3.5</v>
       </c>
       <c r="E41" s="8">
@@ -12205,12 +12210,12 @@
         <v>5</v>
       </c>
       <c r="I41" s="9">
-        <f>('Composite Stats'!$B41+'Composite Stats'!$C41)/2/$H41</f>
-        <v>536.4</v>
+        <f>('Composite Stats'!$B41+'Composite Stats'!$C41+'Base Stat Progression'!$B43+'Base Stat Progression'!$C43)/4/$H41</f>
+        <v>448.4</v>
       </c>
       <c r="J41" s="9">
-        <f>('Composite Stats'!$B41+'Composite Stats'!$C41)/2/$H41*1.5</f>
-        <v>804.59999999999991</v>
+        <f>('Composite Stats'!$B41+'Composite Stats'!$C41+'Base Stat Progression'!$B43+'Base Stat Progression'!$C43)/4/$H41*1.5</f>
+        <v>672.59999999999991</v>
       </c>
       <c r="K41" s="9">
         <f>('Composite Stats'!$B41+'Composite Stats'!$C41)/2/$H41</f>
@@ -12225,17 +12230,17 @@
         <v>52.800000000000011</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>40</v>
       </c>
-      <c r="B42" s="26">
+      <c r="B42" s="25">
         <v>3</v>
       </c>
       <c r="C42" s="4">
         <v>6</v>
       </c>
-      <c r="D42" s="26">
+      <c r="D42" s="25">
         <v>4</v>
       </c>
       <c r="E42" s="8">
@@ -12254,12 +12259,12 @@
         <v>5</v>
       </c>
       <c r="I42" s="9">
-        <f>('Composite Stats'!$B42+'Composite Stats'!$C42)/2/$H42</f>
-        <v>549.20000000000005</v>
+        <f>('Composite Stats'!$B42+'Composite Stats'!$C42+'Base Stat Progression'!$B44+'Base Stat Progression'!$C44)/4/$H42</f>
+        <v>458.95</v>
       </c>
       <c r="J42" s="9">
-        <f>('Composite Stats'!$B42+'Composite Stats'!$C42)/2/$H42*1.5</f>
-        <v>823.80000000000007</v>
+        <f>('Composite Stats'!$B42+'Composite Stats'!$C42+'Base Stat Progression'!$B44+'Base Stat Progression'!$C44)/4/$H42*1.5</f>
+        <v>688.42499999999995</v>
       </c>
       <c r="K42" s="9">
         <f>('Composite Stats'!$B42+'Composite Stats'!$C42)/2/$H42</f>
@@ -12274,17 +12279,17 @@
         <v>53.400000000000013</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10">
         <v>41</v>
       </c>
-      <c r="B43" s="26">
+      <c r="B43" s="25">
         <v>3</v>
       </c>
       <c r="C43" s="4">
         <v>6</v>
       </c>
-      <c r="D43" s="26">
+      <c r="D43" s="25">
         <v>4</v>
       </c>
       <c r="E43" s="8">
@@ -12303,12 +12308,12 @@
         <v>5</v>
       </c>
       <c r="I43" s="9">
-        <f>('Composite Stats'!$B43+'Composite Stats'!$C43)/2/$H43</f>
-        <v>561.99999999999989</v>
+        <f>('Composite Stats'!$B43+'Composite Stats'!$C43+'Base Stat Progression'!$B45+'Base Stat Progression'!$C45)/4/$H43</f>
+        <v>469.49999999999989</v>
       </c>
       <c r="J43" s="9">
-        <f>('Composite Stats'!$B43+'Composite Stats'!$C43)/2/$H43*1.5</f>
-        <v>842.99999999999977</v>
+        <f>('Composite Stats'!$B43+'Composite Stats'!$C43+'Base Stat Progression'!$B45+'Base Stat Progression'!$C45)/4/$H43*1.5</f>
+        <v>704.24999999999977</v>
       </c>
       <c r="K43" s="9">
         <f>('Composite Stats'!$B43+'Composite Stats'!$C43)/2/$H43</f>
@@ -12323,17 +12328,17 @@
         <v>54.000000000000014</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10">
         <v>42</v>
       </c>
-      <c r="B44" s="26">
+      <c r="B44" s="25">
         <v>3</v>
       </c>
       <c r="C44" s="4">
         <v>6</v>
       </c>
-      <c r="D44" s="26">
+      <c r="D44" s="25">
         <v>4</v>
       </c>
       <c r="E44" s="8">
@@ -12352,12 +12357,12 @@
         <v>5</v>
       </c>
       <c r="I44" s="9">
-        <f>('Composite Stats'!$B44+'Composite Stats'!$C44)/2/$H44</f>
-        <v>574.79999999999995</v>
+        <f>('Composite Stats'!$B44+'Composite Stats'!$C44+'Base Stat Progression'!$B46+'Base Stat Progression'!$C46)/4/$H44</f>
+        <v>480.05</v>
       </c>
       <c r="J44" s="9">
-        <f>('Composite Stats'!$B44+'Composite Stats'!$C44)/2/$H44*1.5</f>
-        <v>862.19999999999993</v>
+        <f>('Composite Stats'!$B44+'Composite Stats'!$C44+'Base Stat Progression'!$B46+'Base Stat Progression'!$C46)/4/$H44*1.5</f>
+        <v>720.07500000000005</v>
       </c>
       <c r="K44" s="9">
         <f>('Composite Stats'!$B44+'Composite Stats'!$C44)/2/$H44</f>
@@ -12372,17 +12377,17 @@
         <v>54.600000000000016</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="10">
         <v>43</v>
       </c>
-      <c r="B45" s="26">
+      <c r="B45" s="25">
         <v>3</v>
       </c>
       <c r="C45" s="4">
         <v>6</v>
       </c>
-      <c r="D45" s="26">
+      <c r="D45" s="25">
         <v>4</v>
       </c>
       <c r="E45" s="8">
@@ -12401,12 +12406,12 @@
         <v>5</v>
       </c>
       <c r="I45" s="9">
-        <f>('Composite Stats'!$B45+'Composite Stats'!$C45)/2/$H45</f>
-        <v>587.59999999999991</v>
+        <f>('Composite Stats'!$B45+'Composite Stats'!$C45+'Base Stat Progression'!$B47+'Base Stat Progression'!$C47)/4/$H45</f>
+        <v>490.5999999999998</v>
       </c>
       <c r="J45" s="9">
-        <f>('Composite Stats'!$B45+'Composite Stats'!$C45)/2/$H45*1.5</f>
-        <v>881.39999999999986</v>
+        <f>('Composite Stats'!$B45+'Composite Stats'!$C45+'Base Stat Progression'!$B47+'Base Stat Progression'!$C47)/4/$H45*1.5</f>
+        <v>735.89999999999964</v>
       </c>
       <c r="K45" s="9">
         <f>('Composite Stats'!$B45+'Composite Stats'!$C45)/2/$H45</f>
@@ -12421,17 +12426,17 @@
         <v>55.200000000000017</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10">
         <v>44</v>
       </c>
-      <c r="B46" s="26">
+      <c r="B46" s="25">
         <v>3</v>
       </c>
       <c r="C46" s="4">
         <v>6</v>
       </c>
-      <c r="D46" s="26">
+      <c r="D46" s="25">
         <v>4</v>
       </c>
       <c r="E46" s="8">
@@ -12450,12 +12455,12 @@
         <v>5</v>
       </c>
       <c r="I46" s="9">
-        <f>('Composite Stats'!$B46+'Composite Stats'!$C46)/2/$H46</f>
-        <v>600.4</v>
+        <f>('Composite Stats'!$B46+'Composite Stats'!$C46+'Base Stat Progression'!$B48+'Base Stat Progression'!$C48)/4/$H46</f>
+        <v>501.14999999999992</v>
       </c>
       <c r="J46" s="9">
-        <f>('Composite Stats'!$B46+'Composite Stats'!$C46)/2/$H46*1.5</f>
-        <v>900.59999999999991</v>
+        <f>('Composite Stats'!$B46+'Composite Stats'!$C46+'Base Stat Progression'!$B48+'Base Stat Progression'!$C48)/4/$H46*1.5</f>
+        <v>751.72499999999991</v>
       </c>
       <c r="K46" s="9">
         <f>('Composite Stats'!$B46+'Composite Stats'!$C46)/2/$H46</f>
@@ -12470,17 +12475,17 @@
         <v>55.800000000000018</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="10">
         <v>45</v>
       </c>
-      <c r="B47" s="26">
+      <c r="B47" s="25">
         <v>3</v>
       </c>
       <c r="C47" s="4">
         <v>6</v>
       </c>
-      <c r="D47" s="26">
+      <c r="D47" s="25">
         <v>4.5</v>
       </c>
       <c r="E47" s="8">
@@ -12499,12 +12504,12 @@
         <v>5</v>
       </c>
       <c r="I47" s="9">
-        <f>('Composite Stats'!$B47+'Composite Stats'!$C47)/2/$H47</f>
-        <v>613.19999999999993</v>
+        <f>('Composite Stats'!$B47+'Composite Stats'!$C47+'Base Stat Progression'!$B49+'Base Stat Progression'!$C49)/4/$H47</f>
+        <v>511.69999999999982</v>
       </c>
       <c r="J47" s="9">
-        <f>('Composite Stats'!$B47+'Composite Stats'!$C47)/2/$H47*1.5</f>
-        <v>919.8</v>
+        <f>('Composite Stats'!$B47+'Composite Stats'!$C47+'Base Stat Progression'!$B49+'Base Stat Progression'!$C49)/4/$H47*1.5</f>
+        <v>767.54999999999973</v>
       </c>
       <c r="K47" s="9">
         <f>('Composite Stats'!$B47+'Composite Stats'!$C47)/2/$H47</f>
@@ -12519,17 +12524,17 @@
         <v>56.40000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10">
         <v>46</v>
       </c>
-      <c r="B48" s="26">
+      <c r="B48" s="25">
         <v>3</v>
       </c>
       <c r="C48" s="4">
         <v>6</v>
       </c>
-      <c r="D48" s="26">
+      <c r="D48" s="25">
         <v>4.5</v>
       </c>
       <c r="E48" s="8">
@@ -12548,12 +12553,12 @@
         <v>5</v>
       </c>
       <c r="I48" s="9">
-        <f>('Composite Stats'!$B48+'Composite Stats'!$C48)/2/$H48</f>
-        <v>625.99999999999989</v>
+        <f>('Composite Stats'!$B48+'Composite Stats'!$C48+'Base Stat Progression'!$B50+'Base Stat Progression'!$C50)/4/$H48</f>
+        <v>522.24999999999977</v>
       </c>
       <c r="J48" s="9">
-        <f>('Composite Stats'!$B48+'Composite Stats'!$C48)/2/$H48*1.5</f>
-        <v>938.99999999999977</v>
+        <f>('Composite Stats'!$B48+'Composite Stats'!$C48+'Base Stat Progression'!$B50+'Base Stat Progression'!$C50)/4/$H48*1.5</f>
+        <v>783.37499999999966</v>
       </c>
       <c r="K48" s="9">
         <f>('Composite Stats'!$B48+'Composite Stats'!$C48)/2/$H48</f>
@@ -12568,17 +12573,17 @@
         <v>57.000000000000021</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="10">
         <v>47</v>
       </c>
-      <c r="B49" s="26">
+      <c r="B49" s="25">
         <v>3</v>
       </c>
       <c r="C49" s="4">
         <v>6</v>
       </c>
-      <c r="D49" s="26">
+      <c r="D49" s="25">
         <v>4.5</v>
       </c>
       <c r="E49" s="8">
@@ -12597,12 +12602,12 @@
         <v>5</v>
       </c>
       <c r="I49" s="9">
-        <f>('Composite Stats'!$B49+'Composite Stats'!$C49)/2/$H49</f>
-        <v>638.79999999999984</v>
+        <f>('Composite Stats'!$B49+'Composite Stats'!$C49+'Base Stat Progression'!$B51+'Base Stat Progression'!$C51)/4/$H49</f>
+        <v>532.79999999999984</v>
       </c>
       <c r="J49" s="9">
-        <f>('Composite Stats'!$B49+'Composite Stats'!$C49)/2/$H49*1.5</f>
-        <v>958.19999999999982</v>
+        <f>('Composite Stats'!$B49+'Composite Stats'!$C49+'Base Stat Progression'!$B51+'Base Stat Progression'!$C51)/4/$H49*1.5</f>
+        <v>799.19999999999982</v>
       </c>
       <c r="K49" s="9">
         <f>('Composite Stats'!$B49+'Composite Stats'!$C49)/2/$H49</f>
@@ -12617,17 +12622,17 @@
         <v>57.600000000000023</v>
       </c>
     </row>
-    <row r="50" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10">
         <v>48</v>
       </c>
-      <c r="B50" s="26">
+      <c r="B50" s="25">
         <v>3</v>
       </c>
       <c r="C50" s="4">
         <v>6</v>
       </c>
-      <c r="D50" s="26">
+      <c r="D50" s="25">
         <v>4.5</v>
       </c>
       <c r="E50" s="8">
@@ -12646,12 +12651,12 @@
         <v>5</v>
       </c>
       <c r="I50" s="9">
-        <f>('Composite Stats'!$B50+'Composite Stats'!$C50)/2/$H50</f>
-        <v>651.59999999999991</v>
+        <f>('Composite Stats'!$B50+'Composite Stats'!$C50+'Base Stat Progression'!$B52+'Base Stat Progression'!$C52)/4/$H50</f>
+        <v>543.3499999999998</v>
       </c>
       <c r="J50" s="9">
-        <f>('Composite Stats'!$B50+'Composite Stats'!$C50)/2/$H50*1.5</f>
-        <v>977.39999999999986</v>
+        <f>('Composite Stats'!$B50+'Composite Stats'!$C50+'Base Stat Progression'!$B52+'Base Stat Progression'!$C52)/4/$H50*1.5</f>
+        <v>815.02499999999964</v>
       </c>
       <c r="K50" s="9">
         <f>('Composite Stats'!$B50+'Composite Stats'!$C50)/2/$H50</f>
@@ -12666,17 +12671,17 @@
         <v>58.200000000000024</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="10">
         <v>49</v>
       </c>
-      <c r="B51" s="26">
+      <c r="B51" s="25">
         <v>3</v>
       </c>
       <c r="C51" s="4">
         <v>6</v>
       </c>
-      <c r="D51" s="26">
+      <c r="D51" s="25">
         <v>4.5</v>
       </c>
       <c r="E51" s="8">
@@ -12695,12 +12700,12 @@
         <v>5</v>
       </c>
       <c r="I51" s="9">
-        <f>('Composite Stats'!$B51+'Composite Stats'!$C51)/2/$H51</f>
-        <v>664.39999999999986</v>
+        <f>('Composite Stats'!$B51+'Composite Stats'!$C51+'Base Stat Progression'!$B53+'Base Stat Progression'!$C53)/4/$H51</f>
+        <v>553.89999999999986</v>
       </c>
       <c r="J51" s="9">
-        <f>('Composite Stats'!$B51+'Composite Stats'!$C51)/2/$H51*1.5</f>
-        <v>996.5999999999998</v>
+        <f>('Composite Stats'!$B51+'Composite Stats'!$C51+'Base Stat Progression'!$B53+'Base Stat Progression'!$C53)/4/$H51*1.5</f>
+        <v>830.8499999999998</v>
       </c>
       <c r="K51" s="9">
         <f>('Composite Stats'!$B51+'Composite Stats'!$C51)/2/$H51</f>
@@ -12715,17 +12720,17 @@
         <v>58.800000000000026</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10">
         <v>50</v>
       </c>
-      <c r="B52" s="26">
+      <c r="B52" s="25">
         <v>3</v>
       </c>
       <c r="C52" s="4">
         <v>6</v>
       </c>
-      <c r="D52" s="26">
+      <c r="D52" s="25">
         <v>4.5</v>
       </c>
       <c r="E52" s="8">
@@ -12744,12 +12749,12 @@
         <v>5</v>
       </c>
       <c r="I52" s="9">
-        <f>('Composite Stats'!$B52+'Composite Stats'!$C52)/2/$H52</f>
-        <v>677.19999999999982</v>
+        <f>('Composite Stats'!$B52+'Composite Stats'!$C52+'Base Stat Progression'!$B54+'Base Stat Progression'!$C54)/4/$H52</f>
+        <v>564.44999999999982</v>
       </c>
       <c r="J52" s="9">
-        <f>('Composite Stats'!$B52+'Composite Stats'!$C52)/2/$H52*1.5</f>
-        <v>1015.7999999999997</v>
+        <f>('Composite Stats'!$B52+'Composite Stats'!$C52+'Base Stat Progression'!$B54+'Base Stat Progression'!$C54)/4/$H52*1.5</f>
+        <v>846.67499999999973</v>
       </c>
       <c r="K52" s="9">
         <f>('Composite Stats'!$B52+'Composite Stats'!$C52)/2/$H52</f>
@@ -12764,17 +12769,17 @@
         <v>59.400000000000027</v>
       </c>
     </row>
-    <row r="53" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>51</v>
       </c>
-      <c r="B53" s="26">
+      <c r="B53" s="25">
         <v>3</v>
       </c>
       <c r="C53" s="4">
         <v>7</v>
       </c>
-      <c r="D53" s="26">
+      <c r="D53" s="25">
         <v>4.5</v>
       </c>
       <c r="E53" s="8">
@@ -12793,12 +12798,12 @@
         <v>4</v>
       </c>
       <c r="I53" s="9">
-        <f>('Composite Stats'!$B53+'Composite Stats'!$C53)/2/$H53</f>
-        <v>862.49999999999977</v>
+        <f>('Composite Stats'!$B53+'Composite Stats'!$C53+'Base Stat Progression'!$B55+'Base Stat Progression'!$C55)/4/$H53</f>
+        <v>718.74999999999966</v>
       </c>
       <c r="J53" s="9">
-        <f>('Composite Stats'!$B53+'Composite Stats'!$C53)/2/$H53*1.5</f>
-        <v>1293.7499999999995</v>
+        <f>('Composite Stats'!$B53+'Composite Stats'!$C53+'Base Stat Progression'!$B55+'Base Stat Progression'!$C55)/4/$H53*1.5</f>
+        <v>1078.1249999999995</v>
       </c>
       <c r="K53" s="9">
         <f>('Composite Stats'!$B53+'Composite Stats'!$C53)/2/$H53</f>
@@ -12813,7 +12818,7 @@
         <v>60.000000000000028</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>

</xml_diff>

<commit_message>
More items, a lot of mob item drops, fixed up gold values, and a little more balance.
</commit_message>
<xml_diff>
--- a/Progression.xlsx
+++ b/Progression.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18768" windowHeight="9960" tabRatio="834" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18768" windowHeight="9960" tabRatio="834" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Area Progression" sheetId="1" r:id="rId1"/>
@@ -3852,7 +3852,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3024" topLeftCell="A50" activePane="bottomLeft"/>
       <selection activeCell="K6" sqref="K6"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD24"/>
@@ -10238,18 +10238,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.88671875" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="3.44140625" customWidth="1"/>
+    <col min="4" max="4" width="6.77734375" style="26" customWidth="1"/>
     <col min="5" max="5" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.35">

</xml_diff>